<commit_message>
fix for tc and implement bidirectional relationship among all entities
</commit_message>
<xml_diff>
--- a/issue_list.xlsx
+++ b/issue_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\temp\3\AutomationPortal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8862F011-5BF8-4C49-BB28-A6606D6FBCF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FAC69FB-5993-4ADE-B7A4-C09DF7956E8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{140B35E9-1596-45A3-B2FE-A6E8C4DF2039}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>Need to resolve 500 issues</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>Calling 1 tc in another tc</t>
+  </si>
+  <si>
+    <t>In get modules test cases array displaying twice</t>
   </si>
 </sst>
 </file>
@@ -483,10 +486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1130C8-4123-4C8F-8AF6-726129233EA6}">
-  <dimension ref="B1:C7"/>
+  <dimension ref="B1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,6 +535,11 @@
         <v>10</v>
       </c>
     </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>